<commit_message>
divide create course method
</commit_message>
<xml_diff>
--- a/src/test/resources/MAAssingCourseTests/Upload.xlsx
+++ b/src/test/resources/MAAssingCourseTests/Upload.xlsx
@@ -123,7 +123,7 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -138,7 +138,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>100000002</v>
+        <v>100000003</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>